<commit_message>
bug fix & IP check
</commit_message>
<xml_diff>
--- a/h.xlsx
+++ b/h.xlsx
@@ -505,45 +505,39 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mem:           1,9Gi       1,2Gi       147Mi        10Mi       727Mi       707Mi</t>
+          <t>total : 1,9Gi</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PID COMMAND         %MEM
-   1579 gnome-shell     16.1
-   1805 gnome-software   5.0
-   1789 evolution-alarm  4.6
-   2053 gsd-xsettings    4.0
-   2028 Xwayland         3.3</t>
+          <t>PID: 1579, COMMAND: gnome-shell, %MEM: 16.1
+PID: 1805, COMMAND: gnome-software, %MEM: 5.0
+PID: 1789, COMMAND: evolution-alarm, %MEM: 4.6
+PID: 2053, COMMAND: gsd-xsettings, %MEM: 4.0
+PID: 2028, COMMAND: Xwayland, %MEM: 3.3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>HOME=/home/rudy
-USER=rudy
-PATH=/usr/local/bin:/usr/bin:/bin:/usr/games</t>
+          <t>HOME : /home/rudy
+USER : rudy
+PATH : /usr/local/bin:/usr/bin:/bin:/usr/games</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NAME    SIZE TYPE MOUNTPOINT
-sda      20G disk 
-├─sda1   19G part /
-├─sda2    1K part 
-└─sda5  975M part [SWAP]
-sr0     632M rom</t>
+          <t>NAME: ├─sda1, SIZE: 19G, TYPE: part, MOUNTPOINT: /
+NAME: └─sda5, SIZE: 975M, TYPE: part, MOUNTPOINT: [SWAP]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sys. de fichiers Taille Utilisé Dispo Uti% Monté sur
-udev               934M       0  934M   0% /dev
-tmpfs              194M    1,4M  192M   1% /run
-/dev/sda1           19G    5,3G   13G  30% /
-tmpfs              967M       0  967M   0% /dev/shm
-tmpfs              5,0M    8,0K  5,0M   1% /run/lock
-tmpfs              194M     96K  194M   1% /run/user/1000</t>
+          <t>/dev : {'size': '934M', 'used': '0', 'avail': '934M', 'pcent': '0%'}
+/run : {'size': '194M', 'used': '1,4M', 'avail': '192M', 'pcent': '1%'}
+/ : {'size': '19G', 'used': '5,3G', 'avail': '13G', 'pcent': '30%'}
+/dev/shm : {'size': '967M', 'used': '0', 'avail': '967M', 'pcent': '0%'}
+/run/lock : {'size': '5,0M', 'used': '8,0K', 'avail': '5,0M', 'pcent': '1%'}
+/run/user/1000 : {'size': '194M', 'used': '96K', 'avail': '194M', 'pcent': '1%'}</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">

</xml_diff>